<commit_message>
Timeline shows all the investments in sorted order accprding to dates
</commit_message>
<xml_diff>
--- a/Investments.xlsx
+++ b/Investments.xlsx
@@ -1,27 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr hidePivotFieldList="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CHERRY/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="13840" tabRatio="500"/>
+    <workbookView xWindow="645" yWindow="1185" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Data'!$A$1:$P$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Data'!$A$1:$O$12</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="72">
-  <si>
-    <t>week</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>Category</t>
   </si>
@@ -360,7 +349,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -395,7 +384,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -572,7 +561,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -580,47 +569,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="30" customWidth="1"/>
+    <col min="8" max="8" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>71</v>
-      </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="K1" t="s">
         <v>15</v>
@@ -637,350 +626,314 @@
       <c r="O1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>40695</v>
       </c>
-      <c r="B2" s="1">
-        <v>43252</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2">
+        <v>250</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>250</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>41061</v>
       </c>
-      <c r="B3" s="1">
-        <v>43252</v>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>41791</v>
       </c>
-      <c r="B4" s="1">
-        <v>43252</v>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>14.5</v>
+      </c>
+      <c r="G4" t="s">
         <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4">
-        <v>14.5</v>
       </c>
       <c r="H4" t="s">
         <v>28</v>
       </c>
-      <c r="I4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>41061</v>
       </c>
-      <c r="B5" s="1">
-        <v>43252</v>
+      <c r="B5" t="s">
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="I5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>41426</v>
       </c>
-      <c r="B6" s="1">
-        <v>43252</v>
+      <c r="B6" t="s">
+        <v>34</v>
       </c>
       <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6">
-        <v>40</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="H6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>41061</v>
       </c>
-      <c r="B7" s="1">
-        <v>43252</v>
+      <c r="B7" t="s">
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
         <v>41</v>
       </c>
-      <c r="E7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="I7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>41791</v>
       </c>
-      <c r="B8" s="1">
-        <v>43252</v>
+      <c r="B8" t="s">
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
         <v>46</v>
       </c>
-      <c r="E8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8">
-        <v>15</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I8" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>41426</v>
       </c>
-      <c r="B9" s="1">
-        <v>43252</v>
+      <c r="B9" t="s">
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>48</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <v>10.5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s">
         <v>49</v>
       </c>
-      <c r="F9">
-        <v>10.5</v>
-      </c>
-      <c r="H9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I9" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>41791</v>
       </c>
-      <c r="B10" s="1">
-        <v>43252</v>
+      <c r="B10" t="s">
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
         <v>52</v>
       </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10">
-        <v>11</v>
-      </c>
-      <c r="H10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" t="s">
-        <v>53</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="48" x14ac:dyDescent="0.2">
+      <c r="I10" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>41061</v>
       </c>
-      <c r="B11" s="1">
-        <v>43252</v>
+      <c r="B11" t="s">
+        <v>56</v>
       </c>
       <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11">
-        <v>25</v>
-      </c>
-      <c r="H11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="I11" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>40695</v>
       </c>
-      <c r="B12" s="1">
-        <v>43252</v>
+      <c r="B12" t="s">
+        <v>60</v>
       </c>
       <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="s">
         <v>61</v>
       </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12">
-        <v>7</v>
-      </c>
-      <c r="G12" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="H12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J7" r:id="rId5"/>
-    <hyperlink ref="J6" r:id="rId6"/>
-    <hyperlink ref="J12" r:id="rId7"/>
-    <hyperlink ref="J11" r:id="rId8"/>
-    <hyperlink ref="J10" r:id="rId9"/>
-    <hyperlink ref="J9" r:id="rId10"/>
-    <hyperlink ref="J8" r:id="rId11"/>
-    <hyperlink ref="K2" r:id="rId12"/>
-    <hyperlink ref="I2" r:id="rId13"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I7" r:id="rId5"/>
+    <hyperlink ref="I6" r:id="rId6"/>
+    <hyperlink ref="I12" r:id="rId7"/>
+    <hyperlink ref="I11" r:id="rId8"/>
+    <hyperlink ref="I10" r:id="rId9"/>
+    <hyperlink ref="I9" r:id="rId10"/>
+    <hyperlink ref="I8" r:id="rId11"/>
+    <hyperlink ref="J2" r:id="rId12"/>
+    <hyperlink ref="H2" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>